<commit_message>
added multiple data loadings
</commit_message>
<xml_diff>
--- a/InputData/nst-est2018-01.xlsx
+++ b/InputData/nst-est2018-01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joshi_Pavilion\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DataBootcamp\Projects\GTATL5Project2\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E428D5-15CD-4524-9A4B-530409517DFE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6289B9D-99F7-47A0-A097-1E2AB03C9AE0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NST01" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="68">
   <si>
     <t>United States</t>
   </si>
@@ -63,669 +63,6 @@
     <t>Population Estimate (as of July 1)</t>
   </si>
   <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Alabama</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Alaska</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Arizona</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Arkansas</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>California</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Colorado</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Connecticut</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Delaware</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>District of Columbia</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Florida</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Georgia</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Hawaii</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Idaho</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Illinois</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Indiana</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Iowa</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Kansas</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Kentucky</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Louisiana</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Maine</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Maryland</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Massachusetts</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Michigan</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Minnesota</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Mississippi</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Missouri</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Montana</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Nebraska</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Nevada</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>New Hampshire</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>New Jersey</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>New Mexico</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>New York</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>North Carolina</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>North Dakota</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Ohio</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Oklahoma</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Oregon</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Pennsylvania</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Rhode Island</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>South Carolina</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>South Dakota</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Tennessee</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Texas</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Utah</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Vermont</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Virginia</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Washington</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>West Virginia</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Wisconsin</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Wyoming</t>
-    </r>
-  </si>
-  <si>
     <t>Note: The estimates are based on the 2010 Census and reflect changes to the April 1, 2010 population due to the Count Question Resolution program and geographic program revisions. See Geographic Terms and Definitions at http://www.census.gov/programs-surveys/popest/guidance-geographies/terms-and-definitions.html for a list of the states that are included in each region.  All geographic boundaries for the 2018 population estimates series except statistical area delineations are as of January 1, 2018.  For population estimates methodology statements, see http://www.census.gov/programs-surveys/popest/technical-documentation/methodology.html.</t>
   </si>
   <si>
@@ -739,6 +76,159 @@
   </si>
   <si>
     <t>Release Date: December 2018</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>Delaware</t>
+  </si>
+  <si>
+    <t>District of Columbia</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>Idaho</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>Iowa</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
+    <t>Kentucky</t>
+  </si>
+  <si>
+    <t>Louisiana</t>
+  </si>
+  <si>
+    <t>Maine</t>
+  </si>
+  <si>
+    <t>Maryland</t>
+  </si>
+  <si>
+    <t>Massachusetts</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>Mississippi</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>Montana</t>
+  </si>
+  <si>
+    <t>Nebraska</t>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>New Hampshire</t>
+  </si>
+  <si>
+    <t>New Jersey</t>
+  </si>
+  <si>
+    <t>New Mexico</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>North Dakota</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>Oklahoma</t>
+  </si>
+  <si>
+    <t>Oregon</t>
+  </si>
+  <si>
+    <t>Pennsylvania</t>
+  </si>
+  <si>
+    <t>Rhode Island</t>
+  </si>
+  <si>
+    <t>South Carolina</t>
+  </si>
+  <si>
+    <t>South Dakota</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>Vermont</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>West Virginia</t>
+  </si>
+  <si>
+    <t>Wisconsin</t>
+  </si>
+  <si>
+    <t>Wyoming</t>
   </si>
 </sst>
 </file>
@@ -748,7 +238,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmmm\ d\,\ yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -797,8 +287,13 @@
       <name val="arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="MS sans serif"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -820,6 +315,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1048,6 +549,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="3" fontId="4" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1106,14 +614,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1458,72 +959,72 @@
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A61" sqref="A61"/>
+      <pane ySplit="4" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" style="1" customWidth="1"/>
-    <col min="2" max="11" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" style="1" customWidth="1"/>
+    <col min="2" max="11" width="14.7109375" style="1" customWidth="1"/>
     <col min="12" max="12" width="13" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.109375" style="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="2.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:12" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-    </row>
-    <row r="2" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+    </row>
+    <row r="2" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-    </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+    </row>
+    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="30">
         <v>40269</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="26" t="s">
+      <c r="C3" s="29"/>
+      <c r="D3" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-    </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="25"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+    </row>
+    <row r="4" spans="1:12" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="27"/>
       <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1558,7 +1059,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -1596,7 +1097,7 @@
         <v>327167434</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
@@ -1634,7 +1135,7 @@
         <v>56111079</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
@@ -1672,7 +1173,7 @@
         <v>68308744</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>3</v>
       </c>
@@ -1710,7 +1211,7 @@
         <v>124753948</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>4</v>
       </c>
@@ -1748,9 +1249,9 @@
         <v>77993663</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="32" t="s">
-        <v>12</v>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="34" t="s">
+        <v>17</v>
       </c>
       <c r="B10" s="8">
         <v>4779736</v>
@@ -1782,13 +1283,13 @@
       <c r="K10" s="8">
         <v>4875120</v>
       </c>
-      <c r="L10" s="33">
+      <c r="L10" s="12">
         <v>4887871</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="32" t="s">
-        <v>13</v>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="34" t="s">
+        <v>18</v>
       </c>
       <c r="B11" s="8">
         <v>710231</v>
@@ -1820,13 +1321,13 @@
       <c r="K11" s="8">
         <v>739786</v>
       </c>
-      <c r="L11" s="33">
+      <c r="L11" s="12">
         <v>737438</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="32" t="s">
-        <v>14</v>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="34" t="s">
+        <v>19</v>
       </c>
       <c r="B12" s="8">
         <v>6392017</v>
@@ -1858,13 +1359,13 @@
       <c r="K12" s="8">
         <v>7048876</v>
       </c>
-      <c r="L12" s="33">
+      <c r="L12" s="12">
         <v>7171646</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="32" t="s">
-        <v>15</v>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="34" t="s">
+        <v>20</v>
       </c>
       <c r="B13" s="8">
         <v>2915918</v>
@@ -1896,13 +1397,13 @@
       <c r="K13" s="8">
         <v>3002997</v>
       </c>
-      <c r="L13" s="33">
+      <c r="L13" s="12">
         <v>3013825</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="32" t="s">
-        <v>16</v>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="34" t="s">
+        <v>21</v>
       </c>
       <c r="B14" s="8">
         <v>37253956</v>
@@ -1934,13 +1435,13 @@
       <c r="K14" s="8">
         <v>39399349</v>
       </c>
-      <c r="L14" s="33">
+      <c r="L14" s="12">
         <v>39557045</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="32" t="s">
-        <v>17</v>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="34" t="s">
+        <v>22</v>
       </c>
       <c r="B15" s="8">
         <v>5029196</v>
@@ -1972,13 +1473,13 @@
       <c r="K15" s="8">
         <v>5615902</v>
       </c>
-      <c r="L15" s="33">
+      <c r="L15" s="12">
         <v>5695564</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="32" t="s">
-        <v>18</v>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="34" t="s">
+        <v>23</v>
       </c>
       <c r="B16" s="8">
         <v>3574097</v>
@@ -2010,13 +1511,13 @@
       <c r="K16" s="8">
         <v>3573880</v>
       </c>
-      <c r="L16" s="33">
+      <c r="L16" s="12">
         <v>3572665</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="32" t="s">
-        <v>19</v>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="34" t="s">
+        <v>24</v>
       </c>
       <c r="B17" s="8">
         <v>897934</v>
@@ -2048,13 +1549,13 @@
       <c r="K17" s="8">
         <v>957078</v>
       </c>
-      <c r="L17" s="33">
+      <c r="L17" s="12">
         <v>967171</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="32" t="s">
-        <v>20</v>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="34" t="s">
+        <v>25</v>
       </c>
       <c r="B18" s="8">
         <v>601723</v>
@@ -2086,13 +1587,13 @@
       <c r="K18" s="8">
         <v>695691</v>
       </c>
-      <c r="L18" s="33">
+      <c r="L18" s="12">
         <v>702455</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="32" t="s">
-        <v>21</v>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="34" t="s">
+        <v>26</v>
       </c>
       <c r="B19" s="8">
         <v>18801310</v>
@@ -2124,13 +1625,13 @@
       <c r="K19" s="8">
         <v>20976812</v>
       </c>
-      <c r="L19" s="33">
+      <c r="L19" s="12">
         <v>21299325</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="32" t="s">
-        <v>22</v>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="34" t="s">
+        <v>27</v>
       </c>
       <c r="B20" s="8">
         <v>9687653</v>
@@ -2162,13 +1663,13 @@
       <c r="K20" s="8">
         <v>10413055</v>
       </c>
-      <c r="L20" s="33">
+      <c r="L20" s="12">
         <v>10519475</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="32" t="s">
-        <v>23</v>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="34" t="s">
+        <v>28</v>
       </c>
       <c r="B21" s="8">
         <v>1360301</v>
@@ -2200,13 +1701,13 @@
       <c r="K21" s="8">
         <v>1424203</v>
       </c>
-      <c r="L21" s="33">
+      <c r="L21" s="12">
         <v>1420491</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="32" t="s">
-        <v>24</v>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="34" t="s">
+        <v>29</v>
       </c>
       <c r="B22" s="8">
         <v>1567582</v>
@@ -2238,13 +1739,13 @@
       <c r="K22" s="8">
         <v>1718904</v>
       </c>
-      <c r="L22" s="33">
+      <c r="L22" s="12">
         <v>1754208</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="32" t="s">
-        <v>25</v>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="34" t="s">
+        <v>30</v>
       </c>
       <c r="B23" s="8">
         <v>12830632</v>
@@ -2276,13 +1777,13 @@
       <c r="K23" s="8">
         <v>12786196</v>
       </c>
-      <c r="L23" s="33">
+      <c r="L23" s="12">
         <v>12741080</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="32" t="s">
-        <v>26</v>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="34" t="s">
+        <v>31</v>
       </c>
       <c r="B24" s="8">
         <v>6483802</v>
@@ -2314,13 +1815,13 @@
       <c r="K24" s="8">
         <v>6660082</v>
       </c>
-      <c r="L24" s="33">
+      <c r="L24" s="12">
         <v>6691878</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="32" t="s">
-        <v>27</v>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="34" t="s">
+        <v>32</v>
       </c>
       <c r="B25" s="8">
         <v>3046355</v>
@@ -2352,13 +1853,13 @@
       <c r="K25" s="8">
         <v>3143637</v>
       </c>
-      <c r="L25" s="33">
+      <c r="L25" s="12">
         <v>3156145</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="32" t="s">
-        <v>28</v>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="34" t="s">
+        <v>33</v>
       </c>
       <c r="B26" s="8">
         <v>2853118</v>
@@ -2390,13 +1891,13 @@
       <c r="K26" s="8">
         <v>2910689</v>
       </c>
-      <c r="L26" s="33">
+      <c r="L26" s="12">
         <v>2911505</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="32" t="s">
-        <v>29</v>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="34" t="s">
+        <v>34</v>
       </c>
       <c r="B27" s="8">
         <v>4339367</v>
@@ -2428,13 +1929,13 @@
       <c r="K27" s="8">
         <v>4453874</v>
       </c>
-      <c r="L27" s="33">
+      <c r="L27" s="12">
         <v>4468402</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="32" t="s">
-        <v>30</v>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="34" t="s">
+        <v>35</v>
       </c>
       <c r="B28" s="8">
         <v>4533372</v>
@@ -2466,13 +1967,13 @@
       <c r="K28" s="8">
         <v>4670818</v>
       </c>
-      <c r="L28" s="33">
+      <c r="L28" s="12">
         <v>4659978</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="32" t="s">
-        <v>31</v>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="34" t="s">
+        <v>36</v>
       </c>
       <c r="B29" s="8">
         <v>1328361</v>
@@ -2504,13 +2005,13 @@
       <c r="K29" s="8">
         <v>1335063</v>
       </c>
-      <c r="L29" s="33">
+      <c r="L29" s="12">
         <v>1338404</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="32" t="s">
-        <v>32</v>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="34" t="s">
+        <v>37</v>
       </c>
       <c r="B30" s="8">
         <v>5773552</v>
@@ -2542,13 +2043,13 @@
       <c r="K30" s="8">
         <v>6024891</v>
       </c>
-      <c r="L30" s="33">
+      <c r="L30" s="12">
         <v>6042718</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="32" t="s">
-        <v>33</v>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="34" t="s">
+        <v>38</v>
       </c>
       <c r="B31" s="8">
         <v>6547629</v>
@@ -2580,13 +2081,13 @@
       <c r="K31" s="8">
         <v>6863246</v>
       </c>
-      <c r="L31" s="33">
+      <c r="L31" s="12">
         <v>6902149</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="32" t="s">
-        <v>34</v>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="34" t="s">
+        <v>39</v>
       </c>
       <c r="B32" s="8">
         <v>9883640</v>
@@ -2618,13 +2119,13 @@
       <c r="K32" s="8">
         <v>9976447</v>
       </c>
-      <c r="L32" s="33">
+      <c r="L32" s="12">
         <v>9995915</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="32" t="s">
-        <v>35</v>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="34" t="s">
+        <v>40</v>
       </c>
       <c r="B33" s="8">
         <v>5303925</v>
@@ -2656,13 +2157,13 @@
       <c r="K33" s="8">
         <v>5568155</v>
       </c>
-      <c r="L33" s="33">
+      <c r="L33" s="12">
         <v>5611179</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="32" t="s">
-        <v>36</v>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="34" t="s">
+        <v>41</v>
       </c>
       <c r="B34" s="8">
         <v>2967297</v>
@@ -2694,13 +2195,13 @@
       <c r="K34" s="8">
         <v>2989663</v>
       </c>
-      <c r="L34" s="33">
+      <c r="L34" s="12">
         <v>2986530</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35" s="32" t="s">
-        <v>37</v>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="34" t="s">
+        <v>42</v>
       </c>
       <c r="B35" s="8">
         <v>5988927</v>
@@ -2732,13 +2233,13 @@
       <c r="K35" s="8">
         <v>6108612</v>
       </c>
-      <c r="L35" s="33">
+      <c r="L35" s="12">
         <v>6126452</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="32" t="s">
-        <v>38</v>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="34" t="s">
+        <v>43</v>
       </c>
       <c r="B36" s="8">
         <v>989415</v>
@@ -2770,13 +2271,13 @@
       <c r="K36" s="8">
         <v>1053090</v>
       </c>
-      <c r="L36" s="33">
+      <c r="L36" s="12">
         <v>1062305</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="32" t="s">
-        <v>39</v>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="34" t="s">
+        <v>44</v>
       </c>
       <c r="B37" s="8">
         <v>1826341</v>
@@ -2808,13 +2309,13 @@
       <c r="K37" s="8">
         <v>1917575</v>
       </c>
-      <c r="L37" s="33">
+      <c r="L37" s="12">
         <v>1929268</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="32" t="s">
-        <v>40</v>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="34" t="s">
+        <v>45</v>
       </c>
       <c r="B38" s="8">
         <v>2700551</v>
@@ -2846,13 +2347,13 @@
       <c r="K38" s="8">
         <v>2972405</v>
       </c>
-      <c r="L38" s="33">
+      <c r="L38" s="12">
         <v>3034392</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39" s="32" t="s">
-        <v>41</v>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="34" t="s">
+        <v>46</v>
       </c>
       <c r="B39" s="8">
         <v>1316470</v>
@@ -2884,13 +2385,13 @@
       <c r="K39" s="8">
         <v>1349767</v>
       </c>
-      <c r="L39" s="33">
+      <c r="L39" s="12">
         <v>1356458</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40" s="32" t="s">
-        <v>42</v>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="34" t="s">
+        <v>47</v>
       </c>
       <c r="B40" s="8">
         <v>8791894</v>
@@ -2922,13 +2423,13 @@
       <c r="K40" s="8">
         <v>8888543</v>
       </c>
-      <c r="L40" s="33">
+      <c r="L40" s="12">
         <v>8908520</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A41" s="32" t="s">
-        <v>43</v>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="34" t="s">
+        <v>48</v>
       </c>
       <c r="B41" s="8">
         <v>2059179</v>
@@ -2960,13 +2461,13 @@
       <c r="K41" s="8">
         <v>2093395</v>
       </c>
-      <c r="L41" s="33">
+      <c r="L41" s="12">
         <v>2095428</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" s="32" t="s">
-        <v>44</v>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="34" t="s">
+        <v>49</v>
       </c>
       <c r="B42" s="8">
         <v>19378102</v>
@@ -2998,13 +2499,13 @@
       <c r="K42" s="8">
         <v>19590719</v>
       </c>
-      <c r="L42" s="33">
+      <c r="L42" s="12">
         <v>19542209</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A43" s="32" t="s">
-        <v>45</v>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="34" t="s">
+        <v>50</v>
       </c>
       <c r="B43" s="8">
         <v>9535483</v>
@@ -3036,13 +2537,13 @@
       <c r="K43" s="8">
         <v>10270800</v>
       </c>
-      <c r="L43" s="33">
+      <c r="L43" s="12">
         <v>10383620</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A44" s="32" t="s">
-        <v>46</v>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="34" t="s">
+        <v>51</v>
       </c>
       <c r="B44" s="8">
         <v>672591</v>
@@ -3074,13 +2575,13 @@
       <c r="K44" s="8">
         <v>755176</v>
       </c>
-      <c r="L44" s="33">
+      <c r="L44" s="12">
         <v>760077</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A45" s="32" t="s">
-        <v>47</v>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="34" t="s">
+        <v>52</v>
       </c>
       <c r="B45" s="8">
         <v>11536504</v>
@@ -3112,13 +2613,13 @@
       <c r="K45" s="8">
         <v>11664129</v>
       </c>
-      <c r="L45" s="33">
+      <c r="L45" s="12">
         <v>11689442</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A46" s="32" t="s">
-        <v>48</v>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="34" t="s">
+        <v>53</v>
       </c>
       <c r="B46" s="8">
         <v>3751351</v>
@@ -3150,13 +2651,13 @@
       <c r="K46" s="8">
         <v>3932640</v>
       </c>
-      <c r="L46" s="33">
+      <c r="L46" s="12">
         <v>3943079</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A47" s="32" t="s">
-        <v>49</v>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="34" t="s">
+        <v>54</v>
       </c>
       <c r="B47" s="8">
         <v>3831074</v>
@@ -3188,13 +2689,13 @@
       <c r="K47" s="8">
         <v>4146592</v>
       </c>
-      <c r="L47" s="33">
+      <c r="L47" s="12">
         <v>4190713</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48" s="32" t="s">
-        <v>50</v>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="34" t="s">
+        <v>55</v>
       </c>
       <c r="B48" s="8">
         <v>12702379</v>
@@ -3226,13 +2727,13 @@
       <c r="K48" s="8">
         <v>12790447</v>
       </c>
-      <c r="L48" s="33">
+      <c r="L48" s="12">
         <v>12807060</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A49" s="32" t="s">
-        <v>51</v>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="34" t="s">
+        <v>56</v>
       </c>
       <c r="B49" s="8">
         <v>1052567</v>
@@ -3264,13 +2765,13 @@
       <c r="K49" s="8">
         <v>1056486</v>
       </c>
-      <c r="L49" s="33">
+      <c r="L49" s="12">
         <v>1057315</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A50" s="32" t="s">
-        <v>52</v>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="34" t="s">
+        <v>57</v>
       </c>
       <c r="B50" s="8">
         <v>4625364</v>
@@ -3302,13 +2803,13 @@
       <c r="K50" s="8">
         <v>5021219</v>
       </c>
-      <c r="L50" s="33">
+      <c r="L50" s="12">
         <v>5084127</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A51" s="32" t="s">
-        <v>53</v>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="34" t="s">
+        <v>58</v>
       </c>
       <c r="B51" s="8">
         <v>814180</v>
@@ -3340,13 +2841,13 @@
       <c r="K51" s="8">
         <v>873286</v>
       </c>
-      <c r="L51" s="33">
+      <c r="L51" s="12">
         <v>882235</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A52" s="32" t="s">
-        <v>54</v>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="34" t="s">
+        <v>59</v>
       </c>
       <c r="B52" s="8">
         <v>6346105</v>
@@ -3378,13 +2879,13 @@
       <c r="K52" s="8">
         <v>6708794</v>
       </c>
-      <c r="L52" s="33">
+      <c r="L52" s="12">
         <v>6770010</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A53" s="32" t="s">
-        <v>55</v>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="34" t="s">
+        <v>60</v>
       </c>
       <c r="B53" s="8">
         <v>25145561</v>
@@ -3416,13 +2917,13 @@
       <c r="K53" s="8">
         <v>28322717</v>
       </c>
-      <c r="L53" s="33">
+      <c r="L53" s="12">
         <v>28701845</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A54" s="32" t="s">
-        <v>56</v>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="34" t="s">
+        <v>61</v>
       </c>
       <c r="B54" s="8">
         <v>2763885</v>
@@ -3454,13 +2955,13 @@
       <c r="K54" s="8">
         <v>3103118</v>
       </c>
-      <c r="L54" s="33">
+      <c r="L54" s="12">
         <v>3161105</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A55" s="32" t="s">
-        <v>57</v>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="34" t="s">
+        <v>62</v>
       </c>
       <c r="B55" s="8">
         <v>625741</v>
@@ -3492,13 +2993,13 @@
       <c r="K55" s="8">
         <v>624525</v>
       </c>
-      <c r="L55" s="33">
+      <c r="L55" s="12">
         <v>626299</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A56" s="32" t="s">
-        <v>58</v>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="34" t="s">
+        <v>63</v>
       </c>
       <c r="B56" s="8">
         <v>8001024</v>
@@ -3530,13 +3031,13 @@
       <c r="K56" s="8">
         <v>8465207</v>
       </c>
-      <c r="L56" s="33">
+      <c r="L56" s="12">
         <v>8517685</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A57" s="32" t="s">
-        <v>59</v>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="34" t="s">
+        <v>64</v>
       </c>
       <c r="B57" s="8">
         <v>6724540</v>
@@ -3568,13 +3069,13 @@
       <c r="K57" s="8">
         <v>7425432</v>
       </c>
-      <c r="L57" s="33">
+      <c r="L57" s="12">
         <v>7535591</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A58" s="32" t="s">
-        <v>60</v>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="34" t="s">
+        <v>65</v>
       </c>
       <c r="B58" s="8">
         <v>1852994</v>
@@ -3606,13 +3107,13 @@
       <c r="K58" s="8">
         <v>1817048</v>
       </c>
-      <c r="L58" s="33">
+      <c r="L58" s="12">
         <v>1805832</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A59" s="32" t="s">
-        <v>61</v>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="34" t="s">
+        <v>66</v>
       </c>
       <c r="B59" s="8">
         <v>5686986</v>
@@ -3644,13 +3145,13 @@
       <c r="K59" s="8">
         <v>5792051</v>
       </c>
-      <c r="L59" s="33">
+      <c r="L59" s="12">
         <v>5813568</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A60" s="32" t="s">
-        <v>62</v>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="34" t="s">
+        <v>67</v>
       </c>
       <c r="B60" s="8">
         <v>563626</v>
@@ -3682,12 +3183,12 @@
       <c r="K60" s="8">
         <v>578934</v>
       </c>
-      <c r="L60" s="33">
+      <c r="L60" s="12">
         <v>577737</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A61" s="34"/>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="13"/>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
@@ -3700,7 +3201,7 @@
       <c r="K61" s="8"/>
       <c r="L61" s="8"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
         <v>5</v>
       </c>
@@ -3738,85 +3239,85 @@
         <v>3195153</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="B63" s="30"/>
-      <c r="C63" s="30"/>
-      <c r="D63" s="30"/>
-      <c r="E63" s="30"/>
-      <c r="F63" s="30"/>
-      <c r="G63" s="30"/>
-      <c r="H63" s="30"/>
-      <c r="I63" s="30"/>
-      <c r="J63" s="30"/>
-      <c r="K63" s="30"/>
-      <c r="L63" s="31"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A64" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B64" s="13"/>
-      <c r="C64" s="13"/>
-      <c r="D64" s="13"/>
-      <c r="E64" s="13"/>
-      <c r="F64" s="13"/>
-      <c r="G64" s="13"/>
-      <c r="H64" s="13"/>
-      <c r="I64" s="13"/>
-      <c r="J64" s="13"/>
-      <c r="K64" s="13"/>
-      <c r="L64" s="14"/>
-    </row>
-    <row r="65" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="B65" s="16"/>
-      <c r="C65" s="16"/>
-      <c r="D65" s="16"/>
-      <c r="E65" s="16"/>
-      <c r="F65" s="16"/>
-      <c r="G65" s="16"/>
-      <c r="H65" s="16"/>
-      <c r="I65" s="16"/>
-      <c r="J65" s="16"/>
-      <c r="K65" s="16"/>
-      <c r="L65" s="17"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A66" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="B66" s="16"/>
-      <c r="C66" s="16"/>
-      <c r="D66" s="16"/>
-      <c r="E66" s="16"/>
-      <c r="F66" s="16"/>
-      <c r="G66" s="16"/>
-      <c r="H66" s="16"/>
-      <c r="I66" s="16"/>
-      <c r="J66" s="16"/>
-      <c r="K66" s="16"/>
-      <c r="L66" s="17"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A67" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B67" s="19"/>
-      <c r="C67" s="19"/>
-      <c r="D67" s="19"/>
-      <c r="E67" s="19"/>
-      <c r="F67" s="19"/>
-      <c r="G67" s="19"/>
-      <c r="H67" s="19"/>
-      <c r="I67" s="19"/>
-      <c r="J67" s="19"/>
-      <c r="K67" s="19"/>
-      <c r="L67" s="20"/>
+    <row r="63" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" s="32"/>
+      <c r="C63" s="32"/>
+      <c r="D63" s="32"/>
+      <c r="E63" s="32"/>
+      <c r="F63" s="32"/>
+      <c r="G63" s="32"/>
+      <c r="H63" s="32"/>
+      <c r="I63" s="32"/>
+      <c r="J63" s="32"/>
+      <c r="K63" s="32"/>
+      <c r="L63" s="33"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B64" s="15"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="15"/>
+      <c r="I64" s="15"/>
+      <c r="J64" s="15"/>
+      <c r="K64" s="15"/>
+      <c r="L64" s="16"/>
+    </row>
+    <row r="65" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B65" s="18"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="18"/>
+      <c r="I65" s="18"/>
+      <c r="J65" s="18"/>
+      <c r="K65" s="18"/>
+      <c r="L65" s="19"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B66" s="18"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="18"/>
+      <c r="H66" s="18"/>
+      <c r="I66" s="18"/>
+      <c r="J66" s="18"/>
+      <c r="K66" s="18"/>
+      <c r="L66" s="19"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B67" s="21"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="21"/>
+      <c r="F67" s="21"/>
+      <c r="G67" s="21"/>
+      <c r="H67" s="21"/>
+      <c r="I67" s="21"/>
+      <c r="J67" s="21"/>
+      <c r="K67" s="21"/>
+      <c r="L67" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>